<commit_message>
two new spreadsheets and update to the web page and an update to the spreadsheet template
</commit_message>
<xml_diff>
--- a/test-results/cloudreader/spreadsheets/user-OS-version-browser-date.xlsx
+++ b/test-results/cloudreader/spreadsheets/user-OS-version-browser-date.xlsx
@@ -2735,8 +2735,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="A219" sqref="A219"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="13.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3762,7 +3762,7 @@
         <v>0</v>
       </c>
       <c r="C33" s="22">
-        <f>B33/28</f>
+        <f>B33/29</f>
         <v>0</v>
       </c>
       <c r="D33" s="2"/>

</xml_diff>